<commit_message>
Change column order in built-in linkage map
</commit_message>
<xml_diff>
--- a/data-raw/linkageMap50.xlsx
+++ b/data-raw/linkageMap50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docs\Rstuff\PED_SUITE\shinyapps\klink\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C81632-6AA8-4EBD-A5DB-139DF11F2654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7E822E-323C-46BF-88B8-AA67879B1AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="13656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -558,731 +558,728 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>244.23489000000001</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>244.23489000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>56</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
         <v>1.6660999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>35.058050000000001</v>
+      </c>
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>35.058050000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>90.479029999999995</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>90.479029999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
+      <c r="B6">
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
         <v>223.48320000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>56</v>
+      <c r="B7">
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
         <v>67.178899999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>116.92246</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>116.92246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>157.24131</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>157.24131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>12.9467</v>
+      </c>
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>12.9467</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>56</v>
+      <c r="B11">
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
         <v>156.81292999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>70.320670000000007</v>
+      </c>
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>70.320670000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="B13">
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
         <v>70.320800000000006</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>56</v>
+      <c r="B14">
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
         <v>126.67283999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>56</v>
+      <c r="B15">
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
         <v>154.43395000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>15.772410000000001</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>15.772410000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>56</v>
+      <c r="B17">
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17">
         <v>95.449209999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>118.66248</v>
+      </c>
+      <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>118.66248</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
+      <c r="B19">
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
         <v>36.140709999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>56</v>
+      <c r="B20">
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>7</v>
-      </c>
-      <c r="D20">
         <v>100.2012</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>132.07060000000001</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>132.07060000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>119.96228000000001</v>
+      </c>
+      <c r="D22" t="s">
         <v>57</v>
       </c>
-      <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>119.96228000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>56</v>
+      <c r="B23">
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
         <v>136.44313</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>13</v>
+      <c r="B24">
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
         <v>81.157669999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>3.4018199999999998</v>
+      </c>
+      <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-      <c r="D25">
-        <v>3.4018199999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>28.27346</v>
+      </c>
+      <c r="D26" t="s">
         <v>55</v>
       </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
-        <v>28.27346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>169.89917</v>
+      </c>
+      <c r="D27" t="s">
         <v>58</v>
       </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>169.89917</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
-        <v>56</v>
+      <c r="B28">
+        <v>11</v>
       </c>
       <c r="C28">
-        <v>11</v>
-      </c>
-      <c r="D28">
         <v>4.4893299999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
-        <v>13</v>
+      <c r="B29">
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>11</v>
-      </c>
-      <c r="D29">
         <v>32.888910000000003</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
         <v>31</v>
       </c>
-      <c r="C30">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>117</v>
+      </c>
+      <c r="D31" t="s">
         <v>31</v>
       </c>
-      <c r="C31">
-        <v>11</v>
-      </c>
-      <c r="D31">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
-        <v>56</v>
+      <c r="B32">
+        <v>12</v>
       </c>
       <c r="C32">
-        <v>12</v>
-      </c>
-      <c r="D32">
         <v>15.63031</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>27.571290000000001</v>
+      </c>
+      <c r="D33" t="s">
         <v>58</v>
       </c>
-      <c r="C33">
-        <v>12</v>
-      </c>
-      <c r="D33">
-        <v>27.571290000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34">
         <v>13</v>
       </c>
       <c r="C34">
-        <v>13</v>
-      </c>
-      <c r="D34">
         <v>44.908250000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
-        <v>56</v>
+      <c r="B35">
+        <v>13</v>
       </c>
       <c r="C35">
-        <v>13</v>
-      </c>
-      <c r="D35">
         <v>79.830740000000006</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
-        <v>13</v>
+      <c r="B36">
+        <v>14</v>
       </c>
       <c r="C36">
-        <v>14</v>
-      </c>
-      <c r="D36">
         <v>20.494620000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
-        <v>13</v>
+      <c r="B37">
+        <v>15</v>
       </c>
       <c r="C37">
-        <v>15</v>
-      </c>
-      <c r="D37">
         <v>49.517479999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
-        <v>56</v>
+      <c r="B38">
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>15</v>
-      </c>
-      <c r="D38">
         <v>124.05054</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
         <v>58</v>
       </c>
-      <c r="C39">
-        <v>16</v>
-      </c>
-      <c r="D39">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>14.7</v>
+      </c>
+      <c r="D40" t="s">
         <v>43</v>
       </c>
-      <c r="C40">
-        <v>17</v>
-      </c>
-      <c r="D40">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
-      <c r="B41" t="s">
-        <v>13</v>
+      <c r="B41">
+        <v>17</v>
       </c>
       <c r="C41">
-        <v>17</v>
-      </c>
-      <c r="D41">
         <v>113.11145</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B42" t="s">
-        <v>56</v>
+      <c r="B42">
+        <v>18</v>
       </c>
       <c r="C42">
-        <v>18</v>
-      </c>
-      <c r="D42">
         <v>88.920509999999993</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43" t="s">
-        <v>13</v>
+      <c r="B43">
+        <v>18</v>
       </c>
       <c r="C43">
-        <v>18</v>
-      </c>
-      <c r="D43">
         <v>91.217460000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
-        <v>13</v>
+      <c r="B44">
+        <v>19</v>
       </c>
       <c r="C44">
-        <v>19</v>
-      </c>
-      <c r="D44">
         <v>39.27234</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B45" t="s">
-        <v>56</v>
+      <c r="B45">
+        <v>19</v>
       </c>
       <c r="C45">
-        <v>19</v>
-      </c>
-      <c r="D45">
         <v>51.726179999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" t="s">
-        <v>13</v>
+      <c r="B46">
+        <v>20</v>
       </c>
       <c r="C46">
-        <v>20</v>
-      </c>
-      <c r="D46">
         <v>13.25549</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B47" t="s">
-        <v>56</v>
+      <c r="B47">
+        <v>21</v>
       </c>
       <c r="C47">
-        <v>21</v>
-      </c>
-      <c r="D47">
         <v>14.64555</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>49.464779999999998</v>
+      </c>
+      <c r="D48" t="s">
         <v>57</v>
       </c>
-      <c r="C48">
-        <v>21</v>
-      </c>
-      <c r="D48">
-        <v>49.464779999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
-      <c r="B49" t="s">
-        <v>56</v>
+      <c r="B49">
+        <v>21</v>
       </c>
       <c r="C49">
-        <v>21</v>
-      </c>
-      <c r="D49">
         <v>59.375909999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
-      <c r="B50" t="s">
-        <v>13</v>
+      <c r="B50">
+        <v>22</v>
       </c>
       <c r="C50">
-        <v>22</v>
-      </c>
-      <c r="D50">
         <v>7.3958500000000003</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <v>46.213619999999999</v>
+      </c>
+      <c r="D51" t="s">
         <v>58</v>
-      </c>
-      <c r="C51">
-        <v>22</v>
-      </c>
-      <c r="D51">
-        <v>46.213619999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>